<commit_message>
Added data point to graph
</commit_message>
<xml_diff>
--- a/AStarSearch/TestingData/ExecutionTime.xlsx
+++ b/AStarSearch/TestingData/ExecutionTime.xlsx
@@ -68,7 +68,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="166" formatCode="[h]:mm:ss.000"/>
+    <numFmt numFmtId="165" formatCode="[h]:mm:ss.000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -152,10 +152,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -166,20 +172,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -228,10 +228,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$5</c:f>
+              <c:f>(Sheet1!$B$3:$B$5,Sheet1!$B$9)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>256</c:v>
                 </c:pt>
@@ -240,16 +240,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1296</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$5</c:f>
+              <c:f>(Sheet1!$C$3:$C$5,Sheet1!$C$9)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -258,6 +261,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8920</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8940000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -366,11 +372,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="167406208"/>
-        <c:axId val="167404672"/>
+        <c:axId val="77593984"/>
+        <c:axId val="77603968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="167406208"/>
+        <c:axId val="77593984"/>
         <c:scaling>
           <c:logBase val="4"/>
           <c:orientation val="minMax"/>
@@ -379,12 +385,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167404672"/>
+        <c:crossAx val="77603968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="167404672"/>
+        <c:axId val="77603968"/>
         <c:scaling>
           <c:logBase val="4"/>
           <c:orientation val="minMax"/>
@@ -393,7 +399,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167406208"/>
+        <c:crossAx val="77593984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -412,7 +418,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -741,7 +747,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -754,23 +760,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B1" s="14"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="7" t="s">
+      <c r="H1" s="12"/>
+      <c r="I1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="8"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
@@ -808,20 +814,20 @@
       <c r="A3" s="5">
         <v>4</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="9">
         <f>POWER(A3, 4)</f>
         <v>256</v>
       </c>
       <c r="C3" s="5">
         <v>40</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="9">
         <v>20</v>
       </c>
       <c r="E3" s="5">
         <v>-6</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="10">
         <v>-2</v>
       </c>
       <c r="G3" s="4">
@@ -831,11 +837,11 @@
         <v>-163</v>
       </c>
       <c r="I3" s="2">
-        <f>G3/(POWER($A3,4))</f>
+        <f t="shared" ref="I3:J5" si="0">G3/(POWER($A3,4))</f>
         <v>-1.77734375</v>
       </c>
       <c r="J3">
-        <f>H3/(POWER($A3,4))</f>
+        <f t="shared" si="0"/>
         <v>-0.63671875</v>
       </c>
     </row>
@@ -844,7 +850,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B11" si="0">POWER(A4, 4)</f>
+        <f t="shared" ref="B4:B11" si="1">POWER(A4, 4)</f>
         <v>625</v>
       </c>
       <c r="C4" s="2">
@@ -866,11 +872,11 @@
         <v>-379</v>
       </c>
       <c r="I4" s="2">
-        <f>G4/(POWER($A4,4))</f>
+        <f t="shared" si="0"/>
         <v>-2.3391999999999999</v>
       </c>
       <c r="J4">
-        <f>H4/(POWER($A4,4))</f>
+        <f t="shared" si="0"/>
         <v>-0.60640000000000005</v>
       </c>
     </row>
@@ -879,7 +885,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1296</v>
       </c>
       <c r="C5" s="2">
@@ -901,11 +907,11 @@
         <v>-761</v>
       </c>
       <c r="I5" s="2">
-        <f>G5/(POWER($A5,4))</f>
+        <f t="shared" si="0"/>
         <v>-2.9035493827160495</v>
       </c>
       <c r="J5">
-        <f>H5/(POWER($A5,4))</f>
+        <f t="shared" si="0"/>
         <v>-0.58719135802469136</v>
       </c>
     </row>
@@ -914,7 +920,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2401</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -933,7 +939,7 @@
       </c>
       <c r="I6" s="2"/>
       <c r="J6">
-        <f>H6/(POWER($A6,4))</f>
+        <f t="shared" ref="J6:J11" si="2">H6/(POWER($A6,4))</f>
         <v>-0.57392753019575182</v>
       </c>
     </row>
@@ -942,7 +948,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4096</v>
       </c>
       <c r="C7" s="2"/>
@@ -959,7 +965,7 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7">
-        <f>H7/(POWER($A7,4))</f>
+        <f t="shared" si="2"/>
         <v>-0.564208984375</v>
       </c>
     </row>
@@ -968,7 +974,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6561</v>
       </c>
       <c r="C8" s="2"/>
@@ -985,7 +991,7 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8">
-        <f>H8/(POWER($A8,4))</f>
+        <f t="shared" si="2"/>
         <v>-0.55677488187776258</v>
       </c>
     </row>
@@ -994,7 +1000,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="C9" s="2">
@@ -1013,7 +1019,7 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9">
-        <f>H9/(POWER($A9,4))</f>
+        <f t="shared" si="2"/>
         <v>-0.55089999999999995</v>
       </c>
     </row>
@@ -1022,7 +1028,7 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50625</v>
       </c>
       <c r="C10" s="2"/>
@@ -1039,7 +1045,7 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10">
-        <f>H10/(POWER($A10,4))</f>
+        <f t="shared" si="2"/>
         <v>-0.5336098765432099</v>
       </c>
     </row>
@@ -1048,7 +1054,7 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65536</v>
       </c>
       <c r="C11" s="2"/>
@@ -1065,7 +1071,7 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11">
-        <f>H11/(POWER($A11,4))</f>
+        <f t="shared" si="2"/>
         <v>-0.5314788818359375</v>
       </c>
     </row>
@@ -1094,25 +1100,25 @@
       <c r="I15" s="2"/>
     </row>
     <row r="17" spans="3:5">
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="16"/>
     </row>
     <row r="18" spans="3:5" ht="184.5" customHeight="1">
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="13" t="s">
+      <c r="D18" s="15"/>
+      <c r="E18" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="3:5">
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9"/>
+      <c r="D19" s="13"/>
     </row>
     <row r="20" spans="3:5">
       <c r="D20" s="3"/>

</xml_diff>